<commit_message>
Added tiers to spec
Former-commit-id: e1a7492db741f4dfa47f890cae0df05ed0998642
</commit_message>
<xml_diff>
--- a/Documents/DesignDoc.xlsx
+++ b/Documents/DesignDoc.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>hauteur map</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Settler</t>
+  </si>
+  <si>
+    <t>Tiers</t>
   </si>
 </sst>
 </file>
@@ -121,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +134,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -147,9 +192,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -168,15 +220,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F14" totalsRowShown="0">
-  <autoFilter ref="A1:F14"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:G14" totalsRowShown="0">
+  <autoFilter ref="A1:G14"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Attack Damage"/>
     <tableColumn id="3" name="Attack Range"/>
     <tableColumn id="4" name="Health"/>
     <tableColumn id="5" name="Move Range"/>
     <tableColumn id="6" name="ID"/>
+    <tableColumn id="7" name="Tiers"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -689,10 +742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +757,7 @@
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -723,316 +776,359 @@
       <c r="F1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>50</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
         <v>200</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <f>B2+25</f>
         <v>75</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <f>C$2</f>
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <f>D2+50</f>
         <v>250</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <f>E$2</f>
         <v>2</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <f>B3+25</f>
         <v>100</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <f>C$2</f>
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <f>D3+50</f>
         <v>300</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <f>E$2</f>
         <v>2</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <f>B2</f>
         <v>50</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <f>D2*3/4</f>
         <v>150</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <f>E$2</f>
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <f>B5+25</f>
         <v>75</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <f>C5</f>
         <v>3</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <f>D5+50</f>
         <v>200</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <f>E$2</f>
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <f>B6+25</f>
         <v>100</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <f>C6+1</f>
         <v>4</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <f>D6+50</f>
         <v>250</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <f>E$2</f>
         <v>2</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <f>4*B2</f>
         <v>200</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <f>C$2</f>
         <v>1</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <f>D2*3/4</f>
         <v>150</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <f>E$2+1</f>
         <v>3</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="G8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <f>B8+25</f>
         <v>225</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <f>C8</f>
         <v>1</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <f>D8+50</f>
         <v>200</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <f>E8</f>
         <v>3</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="G9" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>50</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <f>C$2</f>
         <v>1</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <f>D2*1/4+D2</f>
         <v>250</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <f>E$2</f>
         <v>2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="G10" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <f>B10+25</f>
         <v>75</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <f>C$2</f>
         <v>1</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <f>D10+50</f>
         <v>300</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <f>E$2</f>
         <v>2</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="G11" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="6">
         <f>B2*4</f>
         <v>200</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <f>C7</f>
         <v>4</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <f>D2/2</f>
         <v>100</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="G12" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="7">
         <f>B2</f>
         <v>50</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="7">
         <f>C$2</f>
         <v>1</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="7">
         <f>D2*2</f>
         <v>400</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="7">
         <f>E12</f>
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="7">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="G13" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="8">
         <f>B2/10</f>
         <v>5</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="8">
         <f>C$2</f>
         <v>1</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="8">
         <f>D2*1/4</f>
         <v>50</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="8">
         <f>E$2</f>
         <v>2</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="8">
         <v>12</v>
+      </c>
+      <c r="G14" s="8">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Range view to design doc
Former-commit-id: d92f7d27b748f9c3539fe9b131c566ec736a8950
</commit_message>
<xml_diff>
--- a/Documents/DesignDoc.xlsx
+++ b/Documents/DesignDoc.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>hauteur map</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Health</t>
   </si>
   <si>
-    <t>Move Range</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -109,6 +106,12 @@
   </si>
   <si>
     <t>Tiers</t>
+  </si>
+  <si>
+    <t>Action points</t>
+  </si>
+  <si>
+    <t>View Range</t>
   </si>
 </sst>
 </file>
@@ -220,16 +223,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:G14" totalsRowShown="0">
-  <autoFilter ref="A1:G14"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:H14" totalsRowShown="0">
+  <autoFilter ref="A1:H14"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Attack Damage"/>
     <tableColumn id="3" name="Attack Range"/>
     <tableColumn id="4" name="Health"/>
-    <tableColumn id="5" name="Move Range"/>
-    <tableColumn id="6" name="ID"/>
-    <tableColumn id="7" name="Tiers"/>
+    <tableColumn id="5" name="Action points"/>
+    <tableColumn id="6" name="View Range"/>
+    <tableColumn id="7" name="ID"/>
+    <tableColumn id="8" name="Tiers"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -742,10 +746,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,32 +761,35 @@
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="B2" s="2">
         <v>50</v>
@@ -797,15 +804,19 @@
         <v>2</v>
       </c>
       <c r="F2" s="2">
+        <f>Tableau3[[#This Row],[Action points]]+1</f>
+        <v>3</v>
+      </c>
+      <c r="G2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2">
         <f>B2+25</f>
@@ -824,15 +835,19 @@
         <v>2</v>
       </c>
       <c r="F3" s="2">
-        <v>1</v>
+        <f>F$2</f>
+        <v>3</v>
       </c>
       <c r="G3" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2">
         <f>B3+25</f>
@@ -851,15 +866,19 @@
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>2</v>
+        <f>F$2</f>
+        <v>3</v>
       </c>
       <c r="G4" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3">
         <f>B2</f>
@@ -877,15 +896,19 @@
         <v>2</v>
       </c>
       <c r="F5" s="3">
-        <v>3</v>
+        <f>C$5 + 1</f>
+        <v>4</v>
       </c>
       <c r="G5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3">
         <f>B5+25</f>
@@ -904,15 +927,19 @@
         <v>2</v>
       </c>
       <c r="F6" s="3">
+        <f t="shared" ref="F6:F7" si="0">C$5 + 1</f>
         <v>4</v>
       </c>
       <c r="G6" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3">
         <f>B6+25</f>
@@ -931,15 +958,19 @@
         <v>2</v>
       </c>
       <c r="F7" s="3">
+        <f>C$7 + 1</f>
         <v>5</v>
       </c>
       <c r="G7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4">
         <f>4*B2</f>
@@ -958,15 +989,19 @@
         <v>3</v>
       </c>
       <c r="F8" s="4">
+        <f>F$2+1</f>
+        <v>4</v>
+      </c>
+      <c r="G8" s="4">
         <v>6</v>
       </c>
-      <c r="G8" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4">
         <f>B8+25</f>
@@ -985,15 +1020,19 @@
         <v>3</v>
       </c>
       <c r="F9" s="4">
+        <f>F8</f>
+        <v>4</v>
+      </c>
+      <c r="G9" s="4">
         <v>7</v>
       </c>
-      <c r="G9" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="5">
         <v>50</v>
@@ -1011,15 +1050,19 @@
         <v>2</v>
       </c>
       <c r="F10" s="5">
+        <f>F$2</f>
+        <v>3</v>
+      </c>
+      <c r="G10" s="5">
         <v>8</v>
       </c>
-      <c r="G10" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="5">
         <f>B10+25</f>
@@ -1038,15 +1081,19 @@
         <v>2</v>
       </c>
       <c r="F11" s="5">
+        <f>F$2</f>
+        <v>3</v>
+      </c>
+      <c r="G11" s="5">
         <v>9</v>
       </c>
-      <c r="G11" s="5">
+      <c r="H11" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="6">
         <f>B2*4</f>
@@ -1064,15 +1111,19 @@
         <v>1</v>
       </c>
       <c r="F12" s="6">
+        <f>C12+1</f>
+        <v>5</v>
+      </c>
+      <c r="G12" s="6">
         <v>10</v>
       </c>
-      <c r="G12" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="7">
         <f>B2</f>
@@ -1091,15 +1142,19 @@
         <v>1</v>
       </c>
       <c r="F13" s="7">
+        <f>F2</f>
+        <v>3</v>
+      </c>
+      <c r="G13" s="7">
         <v>11</v>
       </c>
-      <c r="G13" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="8">
         <f>B2/10</f>
@@ -1118,9 +1173,13 @@
         <v>2</v>
       </c>
       <c r="F14" s="8">
+        <f>F$2</f>
+        <v>3</v>
+      </c>
+      <c r="G14" s="8">
         <v>12</v>
       </c>
-      <c r="G14" s="8">
+      <c r="H14" s="8">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added range view in Districts
Former-commit-id: 8cb20db213b77e87ad677813b156b8824374d7cd
</commit_message>
<xml_diff>
--- a/Documents/DesignDoc.xlsx
+++ b/Documents/DesignDoc.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>hauteur map</t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>WatchTower</t>
-  </si>
-  <si>
-    <t>?????</t>
   </si>
   <si>
     <t>Inn</t>
@@ -1329,7 +1326,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,7 +1367,7 @@
         <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1395,8 +1392,8 @@
       <c r="G2" s="9">
         <v>0</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>45</v>
+      <c r="H2" s="9">
+        <v>5</v>
       </c>
       <c r="I2" s="9">
         <v>0</v>
@@ -1425,8 +1422,8 @@
       <c r="G3" s="6">
         <v>0</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>45</v>
+      <c r="H3" s="6">
+        <v>3</v>
       </c>
       <c r="I3" s="6">
         <v>1</v>
@@ -1455,8 +1452,8 @@
       <c r="G4" s="6">
         <v>0</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>45</v>
+      <c r="H4" s="6">
+        <v>4</v>
       </c>
       <c r="I4" s="6">
         <v>2</v>
@@ -1485,8 +1482,8 @@
       <c r="G5" s="6">
         <v>0</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>45</v>
+      <c r="H5" s="6">
+        <v>5</v>
       </c>
       <c r="I5" s="6">
         <v>3</v>
@@ -1515,8 +1512,8 @@
       <c r="G6" s="1">
         <v>75</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>45</v>
+      <c r="H6" s="1">
+        <v>3</v>
       </c>
       <c r="I6" s="1">
         <v>4</v>
@@ -1545,8 +1542,8 @@
       <c r="G7" s="1">
         <v>100</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>45</v>
+      <c r="H7" s="1">
+        <v>4</v>
       </c>
       <c r="I7" s="1">
         <v>5</v>
@@ -1575,8 +1572,8 @@
       <c r="G8" s="1">
         <v>175</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>45</v>
+      <c r="H8" s="1">
+        <v>5</v>
       </c>
       <c r="I8" s="1">
         <v>6</v>
@@ -1605,8 +1602,8 @@
       <c r="G9" s="8">
         <v>0</v>
       </c>
-      <c r="H9" s="8" t="s">
-        <v>45</v>
+      <c r="H9" s="8">
+        <v>3</v>
       </c>
       <c r="I9" s="8">
         <v>7</v>
@@ -1635,8 +1632,8 @@
       <c r="G10" s="8">
         <v>0</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>45</v>
+      <c r="H10" s="8">
+        <v>4</v>
       </c>
       <c r="I10" s="8">
         <v>8</v>
@@ -1665,8 +1662,8 @@
       <c r="G11" s="8">
         <v>0</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>45</v>
+      <c r="H11" s="8">
+        <v>5</v>
       </c>
       <c r="I11" s="8">
         <v>9</v>
@@ -1695,8 +1692,8 @@
       <c r="G12" s="7">
         <v>0</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>45</v>
+      <c r="H12" s="7">
+        <v>5</v>
       </c>
       <c r="I12" s="7">
         <v>10</v>
@@ -1705,7 +1702,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="11">
         <v>25</v>
@@ -1725,8 +1722,8 @@
       <c r="G13" s="11">
         <v>0</v>
       </c>
-      <c r="H13" s="11" t="s">
-        <v>45</v>
+      <c r="H13" s="11">
+        <v>4</v>
       </c>
       <c r="I13" s="11">
         <v>11</v>
@@ -1735,7 +1732,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="10">
         <v>25</v>
@@ -1755,8 +1752,8 @@
       <c r="G14" s="10">
         <v>100</v>
       </c>
-      <c r="H14" s="10" t="s">
-        <v>45</v>
+      <c r="H14" s="10">
+        <v>4</v>
       </c>
       <c r="I14" s="10">
         <v>12</v>
@@ -1765,7 +1762,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="12">
         <v>75</v>
@@ -1785,19 +1782,19 @@
       <c r="G15" s="12">
         <v>0</v>
       </c>
-      <c r="H15" s="12" t="s">
-        <v>45</v>
+      <c r="H15" s="12">
+        <v>5</v>
       </c>
       <c r="I15" s="12">
         <v>13</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="12">
         <v>75</v>
@@ -1817,19 +1814,19 @@
       <c r="G16" s="12">
         <v>0</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>45</v>
+      <c r="H16" s="12">
+        <v>5</v>
       </c>
       <c r="I16" s="12">
         <v>14</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="12">
         <v>75</v>
@@ -1849,19 +1846,19 @@
       <c r="G17" s="12">
         <v>0</v>
       </c>
-      <c r="H17" s="12" t="s">
-        <v>45</v>
+      <c r="H17" s="12">
+        <v>5</v>
       </c>
       <c r="I17" s="12">
         <v>15</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="12">
         <v>100</v>
@@ -1881,14 +1878,14 @@
       <c r="G18" s="12">
         <v>0</v>
       </c>
-      <c r="H18" s="12" t="s">
-        <v>45</v>
+      <c r="H18" s="12">
+        <v>5</v>
       </c>
       <c r="I18" s="12">
         <v>16</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>